<commit_message>
se sube para emitir las pólizas de movilidad en QA
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Accesorios.xlsx
+++ b/Sura/DataSource - Accesorios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272EF117-D87C-491D-9E45-055FF247F5E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84B5AE0-EB9B-46AC-8CD1-1B6B4FFDCFEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>Malacate</t>
   </si>
   <si>
-    <t>Hasta $20.000</t>
-  </si>
-  <si>
     <t>NombreAccesorios</t>
   </si>
   <si>
     <t>SumaAseguradaAcce</t>
+  </si>
+  <si>
+    <t>Hasta $150.000</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,10 +389,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -400,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se sube arreglo de Recording Emision/EmisionPoliza.rxrec y Emision/Comisiones.UserCode.cs para que detecte el item Movilidad
</commit_message>
<xml_diff>
--- a/Sura/DataSource - Accesorios.xlsx
+++ b/Sura/DataSource - Accesorios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\Sura\Sura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84B5AE0-EB9B-46AC-8CD1-1B6B4FFDCFEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382D693A-F9F0-4CD5-99C2-F0C965E00E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,24 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Movilidad</t>
-  </si>
-  <si>
-    <t>Aire Acondicionado</t>
-  </si>
-  <si>
-    <t>Reproductores de Sonido</t>
-  </si>
-  <si>
-    <t>Malacate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>NombreAccesorios</t>
   </si>
   <si>
     <t>SumaAseguradaAcce</t>
+  </si>
+  <si>
+    <t>Movilidad</t>
   </si>
   <si>
     <t>Hasta $150.000</t>
@@ -372,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,32 +380,17 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>